<commit_message>
Remover serviceAccountKey.json del repo y agregar al gitignore
</commit_message>
<xml_diff>
--- a/subir/Listado de productos - 3.xlsx
+++ b/subir/Listado de productos - 3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t xml:space="preserve">Codigo</t>
   </si>
@@ -58,22 +58,25 @@
     <t xml:space="preserve">Stock</t>
   </si>
   <si>
-    <t xml:space="preserve">ECKL202734</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBO AMOLADORA + TALADRO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMTOP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inalambrico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBO2</t>
+    <t xml:space="preserve">ETCS0702</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GABINETE PORTA HERRAMIENTAS 7 CAJONES  vacio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMTOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TALADRO PERCUTOR 20V 13MM 20V 96NM SIN CARBONES SIN BAT. NI CARGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ingco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLAVE DE IMPACTO 20V 3/4" 1350NM-SIN CARBONES-SIN BAT. NI CARGADOR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARGADOR RAPIDO BATERIAS 2.0 AH + 1 BATERIA 4AH</t>
   </si>
 </sst>
 </file>
@@ -82,7 +85,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00\ %"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -182,7 +185,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -207,8 +210,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -349,12 +360,17 @@
   <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="1" style="1" width="23.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="73.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="6" style="1" width="23.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="15.16"/>
   </cols>
   <sheetData>
@@ -398,359 +414,416 @@
       <c r="M1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="8" t="n">
+        <v>546952</v>
+      </c>
+      <c r="G2" s="9" t="n">
+        <f aca="false">F2*1.5</f>
+        <v>820428</v>
+      </c>
+      <c r="H2" s="9" t="n">
+        <f aca="false">G2*1.065</f>
+        <v>873755.82</v>
+      </c>
+      <c r="I2" s="9" t="n">
+        <f aca="false">H2*1.3</f>
+        <v>1135882.566</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="n">
+        <v>209681</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="7" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="F2" s="3" t="n">
-        <v>197246</v>
-      </c>
-      <c r="G2" s="3" t="n">
-        <f aca="false">F2*1.5</f>
-        <v>295869</v>
-      </c>
-      <c r="H2" s="3" t="n">
-        <f aca="false">G2*1.065</f>
-        <v>315100.485</v>
-      </c>
-      <c r="I2" s="3" t="n">
-        <f aca="false">H2*1.3</f>
-        <v>409630.6305</v>
-      </c>
-      <c r="J2" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="M2" s="5"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="F3" s="8" t="n">
+        <v>92535</v>
+      </c>
+      <c r="G3" s="9" t="n">
+        <f aca="false">F3*1.5</f>
+        <v>138802.5</v>
+      </c>
+      <c r="H3" s="9" t="n">
+        <f aca="false">G3*1.065</f>
+        <v>147824.6625</v>
+      </c>
+      <c r="I3" s="9" t="n">
+        <f aca="false">H3*1.3</f>
+        <v>192172.06125</v>
+      </c>
+      <c r="J3" s="6" t="n">
+        <v>209681</v>
+      </c>
+      <c r="K3" s="6" t="n">
+        <v>209681</v>
+      </c>
       <c r="L3" s="4"/>
       <c r="M3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="A4" s="6" t="n">
+        <v>201351</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="F4" s="8" t="n">
+        <v>334000</v>
+      </c>
+      <c r="G4" s="9" t="n">
+        <f aca="false">F4*1.5</f>
+        <v>501000</v>
+      </c>
+      <c r="H4" s="9" t="n">
+        <f aca="false">G4*1.065</f>
+        <v>533565</v>
+      </c>
+      <c r="I4" s="9" t="n">
+        <f aca="false">H4*1.3</f>
+        <v>693634.5</v>
+      </c>
+      <c r="J4" s="6" t="n">
+        <v>201351</v>
+      </c>
+      <c r="K4" s="6" t="n">
+        <v>201351</v>
+      </c>
       <c r="L4" s="4"/>
       <c r="M4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="A5" s="6" t="n">
+        <v>12144</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="F5" s="8" t="n">
+        <v>60400</v>
+      </c>
+      <c r="G5" s="9" t="n">
+        <f aca="false">F5*1.5</f>
+        <v>90600</v>
+      </c>
+      <c r="H5" s="9" t="n">
+        <f aca="false">G5*1.065</f>
+        <v>96489</v>
+      </c>
+      <c r="I5" s="9" t="n">
+        <f aca="false">H5*1.3</f>
+        <v>125435.7</v>
+      </c>
+      <c r="J5" s="6" t="n">
+        <v>12144</v>
+      </c>
+      <c r="K5" s="6" t="n">
+        <v>12144</v>
+      </c>
       <c r="L5" s="4"/>
       <c r="M5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
       <c r="L6" s="4"/>
       <c r="M6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
       <c r="L7" s="4"/>
       <c r="M7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="4"/>
       <c r="M8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
     </row>
@@ -786,9 +859,9 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
-      <c r="B26" s="8"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="8"/>
+      <c r="D26" s="10"/>
       <c r="E26" s="5"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -965,79 +1038,79 @@
       <c r="M37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="9"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="9"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="9"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="9"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>